<commit_message>
Update DSM Scheduled Flights vs actual.xlsx
</commit_message>
<xml_diff>
--- a/codeLibrary/R/R/airlineData/DSM Scheduled Flights vs actual.xlsx
+++ b/codeLibrary/R/R/airlineData/DSM Scheduled Flights vs actual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Sites/LVM-Code/codeLibrary/R/R/airlineData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D634741-F79C-CA43-9039-BA181482A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C320D216-56E4-764F-8ECF-08709665BB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="1180" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="659">
   <si>
     <t>DateTime</t>
   </si>
@@ -1980,6 +1980,33 @@
   </si>
   <si>
     <t>2022-01-14</t>
+  </si>
+  <si>
+    <t>2022-01-15</t>
+  </si>
+  <si>
+    <t>2022-01-16</t>
+  </si>
+  <si>
+    <t>2022-01-17</t>
+  </si>
+  <si>
+    <t>2022-01-18</t>
+  </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
+  <si>
+    <t>2022-01-20</t>
+  </si>
+  <si>
+    <t>2022-01-21</t>
+  </si>
+  <si>
+    <t>2022-01-22</t>
+  </si>
+  <si>
+    <t>2022-01-23</t>
   </si>
 </sst>
 </file>
@@ -2858,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K649"/>
+  <dimension ref="A1:K658"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A615" workbookViewId="0">
-      <selection activeCell="F647" sqref="F647"/>
+      <selection activeCell="G655" sqref="G655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12517,7 +12544,7 @@
         <v>44</v>
       </c>
       <c r="D643" s="3">
-        <f t="shared" ref="D643:D649" si="10">C643/B643</f>
+        <f t="shared" ref="D643:D658" si="10">C643/B643</f>
         <v>0.91666666666666663</v>
       </c>
     </row>
@@ -12609,6 +12636,141 @@
       <c r="D649" s="3">
         <f t="shared" si="10"/>
         <v>0.89655172413793105</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A650" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B650" s="2">
+        <v>50</v>
+      </c>
+      <c r="C650" s="2">
+        <v>41</v>
+      </c>
+      <c r="D650" s="3">
+        <f t="shared" si="10"/>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A651" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B651" s="2">
+        <v>53</v>
+      </c>
+      <c r="C651" s="2">
+        <v>48</v>
+      </c>
+      <c r="D651" s="3">
+        <f t="shared" si="10"/>
+        <v>0.90566037735849059</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A652" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B652" s="2">
+        <v>60</v>
+      </c>
+      <c r="C652" s="2">
+        <v>54</v>
+      </c>
+      <c r="D652" s="3">
+        <f t="shared" si="10"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A653" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B653" s="2">
+        <v>55</v>
+      </c>
+      <c r="C653" s="2">
+        <v>54</v>
+      </c>
+      <c r="D653" s="3">
+        <f t="shared" si="10"/>
+        <v>0.98181818181818181</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A654" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B654" s="2">
+        <v>55</v>
+      </c>
+      <c r="C654" s="2">
+        <v>51</v>
+      </c>
+      <c r="D654" s="3">
+        <f t="shared" si="10"/>
+        <v>0.92727272727272725</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A655" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B655" s="2">
+        <v>75</v>
+      </c>
+      <c r="C655" s="2">
+        <v>71</v>
+      </c>
+      <c r="D655" s="3">
+        <f t="shared" si="10"/>
+        <v>0.94666666666666666</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A656" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B656" s="2">
+        <v>70</v>
+      </c>
+      <c r="C656" s="2">
+        <v>66</v>
+      </c>
+      <c r="D656" s="3">
+        <f t="shared" si="10"/>
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A657" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B657" s="2">
+        <v>48</v>
+      </c>
+      <c r="C657" s="2">
+        <v>43</v>
+      </c>
+      <c r="D657" s="3">
+        <f t="shared" si="10"/>
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A658" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B658" s="2">
+        <v>57</v>
+      </c>
+      <c r="C658" s="2">
+        <v>54</v>
+      </c>
+      <c r="D658" s="3">
+        <f t="shared" si="10"/>
+        <v>0.94736842105263153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated air traffric data
</commit_message>
<xml_diff>
--- a/codeLibrary/R/R/airlineData/DSM Scheduled Flights vs actual.xlsx
+++ b/codeLibrary/R/R/airlineData/DSM Scheduled Flights vs actual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Sites/LVM-Code/codeLibrary/R/R/airlineData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD4A82-3EAB-6847-B8F0-0C568854C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A2BE3-6F90-0E44-9EF6-99A1D5FFFE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -926,7 +926,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -934,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D969"/>
+  <dimension ref="A1:D991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A929" workbookViewId="0">
-      <selection activeCell="E967" sqref="E967"/>
+    <sheetView tabSelected="1" topLeftCell="A953" workbookViewId="0">
+      <selection activeCell="F984" sqref="F984"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15342,7 +15342,7 @@
         <v>62</v>
       </c>
       <c r="D960" s="1">
-        <f t="shared" ref="D960:D969" si="15">C960/B960</f>
+        <f t="shared" ref="D960:D991" si="15">C960/B960</f>
         <v>1</v>
       </c>
     </row>
@@ -15479,6 +15479,336 @@
       <c r="D969" s="1">
         <f t="shared" si="15"/>
         <v>0.95890410958904104</v>
+      </c>
+    </row>
+    <row r="970" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A970" s="9">
+        <v>44898</v>
+      </c>
+      <c r="B970" s="10">
+        <v>48</v>
+      </c>
+      <c r="C970" s="10">
+        <v>48</v>
+      </c>
+      <c r="D970" s="1">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="971" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A971" s="9">
+        <v>44899</v>
+      </c>
+      <c r="B971" s="10">
+        <v>63</v>
+      </c>
+      <c r="C971" s="10">
+        <v>63</v>
+      </c>
+      <c r="D971" s="1">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="972" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A972" s="9">
+        <v>44900</v>
+      </c>
+      <c r="B972" s="10">
+        <v>66</v>
+      </c>
+      <c r="C972" s="10">
+        <v>63</v>
+      </c>
+      <c r="D972" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95454545454545459</v>
+      </c>
+    </row>
+    <row r="973" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A973" s="9">
+        <v>44901</v>
+      </c>
+      <c r="B973" s="10">
+        <v>75</v>
+      </c>
+      <c r="C973" s="10">
+        <v>72</v>
+      </c>
+      <c r="D973" s="1">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="974" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A974" s="9">
+        <v>44902</v>
+      </c>
+      <c r="B974" s="10">
+        <v>74</v>
+      </c>
+      <c r="C974" s="10">
+        <v>69</v>
+      </c>
+      <c r="D974" s="1">
+        <f t="shared" si="15"/>
+        <v>0.93243243243243246</v>
+      </c>
+    </row>
+    <row r="975" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A975" s="9">
+        <v>44903</v>
+      </c>
+      <c r="B975" s="10">
+        <v>83</v>
+      </c>
+      <c r="C975" s="10">
+        <v>77</v>
+      </c>
+      <c r="D975" s="1">
+        <f t="shared" si="15"/>
+        <v>0.92771084337349397</v>
+      </c>
+    </row>
+    <row r="976" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A976" s="9">
+        <v>44904</v>
+      </c>
+      <c r="B976" s="10">
+        <v>66</v>
+      </c>
+      <c r="C976" s="10">
+        <v>62</v>
+      </c>
+      <c r="D976" s="1">
+        <f t="shared" si="15"/>
+        <v>0.93939393939393945</v>
+      </c>
+    </row>
+    <row r="977" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A977" s="9">
+        <v>44905</v>
+      </c>
+      <c r="B977" s="10">
+        <v>50</v>
+      </c>
+      <c r="C977" s="10">
+        <v>48</v>
+      </c>
+      <c r="D977" s="1">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="978" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A978" s="9">
+        <v>44906</v>
+      </c>
+      <c r="B978" s="10">
+        <v>60</v>
+      </c>
+      <c r="C978" s="10">
+        <v>59</v>
+      </c>
+      <c r="D978" s="1">
+        <f t="shared" si="15"/>
+        <v>0.98333333333333328</v>
+      </c>
+    </row>
+    <row r="979" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A979" s="9">
+        <v>44907</v>
+      </c>
+      <c r="B979" s="10">
+        <v>68</v>
+      </c>
+      <c r="C979" s="10">
+        <v>67</v>
+      </c>
+      <c r="D979" s="1">
+        <f t="shared" si="15"/>
+        <v>0.98529411764705888</v>
+      </c>
+    </row>
+    <row r="980" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A980" s="9">
+        <v>44908</v>
+      </c>
+      <c r="B980" s="10">
+        <v>63</v>
+      </c>
+      <c r="C980" s="10">
+        <v>58</v>
+      </c>
+      <c r="D980" s="1">
+        <f t="shared" si="15"/>
+        <v>0.92063492063492058</v>
+      </c>
+    </row>
+    <row r="981" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A981" s="9">
+        <v>44909</v>
+      </c>
+      <c r="B981" s="10">
+        <v>65</v>
+      </c>
+      <c r="C981" s="10">
+        <v>64</v>
+      </c>
+      <c r="D981" s="1">
+        <f t="shared" si="15"/>
+        <v>0.98461538461538467</v>
+      </c>
+    </row>
+    <row r="982" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A982" s="9">
+        <v>44910</v>
+      </c>
+      <c r="B982" s="10">
+        <v>72</v>
+      </c>
+      <c r="C982" s="10">
+        <v>67</v>
+      </c>
+      <c r="D982" s="1">
+        <f t="shared" si="15"/>
+        <v>0.93055555555555558</v>
+      </c>
+    </row>
+    <row r="983" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A983" s="9">
+        <v>44911</v>
+      </c>
+      <c r="B983" s="10">
+        <v>78</v>
+      </c>
+      <c r="C983" s="10">
+        <v>76</v>
+      </c>
+      <c r="D983" s="1">
+        <f t="shared" si="15"/>
+        <v>0.97435897435897434</v>
+      </c>
+    </row>
+    <row r="984" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A984" s="9">
+        <v>44912</v>
+      </c>
+      <c r="B984" s="10">
+        <v>52</v>
+      </c>
+      <c r="C984" s="10">
+        <v>51</v>
+      </c>
+      <c r="D984" s="1">
+        <f t="shared" si="15"/>
+        <v>0.98076923076923073</v>
+      </c>
+    </row>
+    <row r="985" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A985" s="9">
+        <v>44913</v>
+      </c>
+      <c r="B985" s="10">
+        <v>55</v>
+      </c>
+      <c r="C985" s="10">
+        <v>53</v>
+      </c>
+      <c r="D985" s="1">
+        <f t="shared" si="15"/>
+        <v>0.96363636363636362</v>
+      </c>
+    </row>
+    <row r="986" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A986" s="9">
+        <v>44914</v>
+      </c>
+      <c r="B986" s="10">
+        <v>56</v>
+      </c>
+      <c r="C986" s="10">
+        <v>54</v>
+      </c>
+      <c r="D986" s="1">
+        <f t="shared" si="15"/>
+        <v>0.9642857142857143</v>
+      </c>
+    </row>
+    <row r="987" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A987" s="9">
+        <v>44915</v>
+      </c>
+      <c r="B987" s="10">
+        <v>76</v>
+      </c>
+      <c r="C987" s="10">
+        <v>72</v>
+      </c>
+      <c r="D987" s="1">
+        <f t="shared" si="15"/>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="988" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A988" s="9">
+        <v>44916</v>
+      </c>
+      <c r="B988" s="10">
+        <v>73</v>
+      </c>
+      <c r="C988" s="10">
+        <v>63</v>
+      </c>
+      <c r="D988" s="1">
+        <f t="shared" si="15"/>
+        <v>0.86301369863013699</v>
+      </c>
+    </row>
+    <row r="989" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A989" s="9">
+        <v>44917</v>
+      </c>
+      <c r="B989" s="10">
+        <v>62</v>
+      </c>
+      <c r="C989" s="10">
+        <v>45</v>
+      </c>
+      <c r="D989" s="1">
+        <f t="shared" si="15"/>
+        <v>0.72580645161290325</v>
+      </c>
+    </row>
+    <row r="990" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A990" s="9">
+        <v>44918</v>
+      </c>
+      <c r="B990" s="10">
+        <v>57</v>
+      </c>
+      <c r="C990" s="10">
+        <v>35</v>
+      </c>
+      <c r="D990" s="1">
+        <f t="shared" si="15"/>
+        <v>0.61403508771929827</v>
+      </c>
+    </row>
+    <row r="991" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A991" s="9">
+        <v>44919</v>
+      </c>
+      <c r="B991" s="10">
+        <v>53</v>
+      </c>
+      <c r="C991" s="10">
+        <v>41</v>
+      </c>
+      <c r="D991" s="1">
+        <f t="shared" si="15"/>
+        <v>0.77358490566037741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>